<commit_message>
Implemented decode and encode to base64
</commit_message>
<xml_diff>
--- a/Data/dataArchive.xlsx
+++ b/Data/dataArchive.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>usuario</t>
   </si>
@@ -24,15 +24,38 @@
     <t>contraseña</t>
   </si>
   <si>
-    <t>prueba</t>
+    <t>MWEyUzNkNEZ0ZXN0UGFzc3dvcmQ=</t>
+  </si>
+  <si>
+    <t>MXEyVzNlNFJ0ZXN0UGFzc3dvcmQ=</t>
+  </si>
+  <si>
+    <t>dXN1YXJpb1BydWViYQ==</t>
+  </si>
+  <si>
+    <t>dXN1YXJpb1Bpenph</t>
+  </si>
+  <si>
+    <t>dXN1YXJpb0NhcGliYXJh</t>
+  </si>
+  <si>
+    <t>OU04bjdCNnZ0ZXN0UGFzc3dvcmQ=</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -60,8 +83,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -365,16 +391,16 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -382,18 +408,18 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>